<commit_message>
Change ntc to correct order
</commit_message>
<xml_diff>
--- a/SeminarPaper/Model/input_data/ntc.xlsx
+++ b/SeminarPaper/Model/input_data/ntc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDC21A5-9C60-41D8-A020-12FABCB5279A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86987AD-EB41-44D8-9A14-D327F6C0EA06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,24 +211,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -253,6 +235,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -537,40 +537,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="8"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="9"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,223 +595,223 @@
       <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7">
         <v>1500</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6">
         <v>1426</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="14"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
         <v>1091.25</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="14"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="6">
         <v>2600</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6">
         <v>1800</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="15">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="9">
         <v>1241.6666666666599</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="8">
         <v>2000</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6">
         <v>2075</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="6">
         <v>1675</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="12">
+      <c r="F7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="6">
         <v>980</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="6">
         <v>2850</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="14"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
         <v>980</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="14"/>
+      <c r="G8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="12">
         <v>1426</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
         <v>2400</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="14">
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="8">
         <v>1016</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="12">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="6">
         <v>1500</v>
       </c>
-      <c r="K10" s="14"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="15">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="9">
         <v>1070.8333333333301</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
         <v>1468.75</v>
       </c>
-      <c r="J11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="14"/>
+      <c r="J11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10">
         <v>2000</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10">
         <v>1016</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17" t="s">
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="9"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
@@ -822,165 +822,165 @@
         <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="20">
-        <v>0</v>
-      </c>
-      <c r="E17" s="20">
+      <c r="C17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
         <f>F5</f>
         <v>1091.25</v>
       </c>
-      <c r="F17" s="20">
-        <v>0</v>
-      </c>
-      <c r="G17" s="20">
-        <v>0</v>
-      </c>
-      <c r="H17" s="21">
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14">
+        <v>0</v>
+      </c>
+      <c r="H17" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="20">
-        <v>0</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="20">
+      <c r="C18" s="14">
+        <v>0</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="14">
         <f>F6</f>
         <v>1800</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="16">
+        <f>J6</f>
+        <v>1241.6666666666599</v>
+      </c>
+      <c r="G18" s="14">
         <f>C6+G6+H6</f>
         <v>2600</v>
       </c>
-      <c r="G18" s="22">
-        <f>J6</f>
-        <v>1241.6666666666599</v>
-      </c>
-      <c r="H18" s="21">
+      <c r="H18" s="15">
         <f>K6</f>
         <v>2000</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="14">
         <f>D7</f>
         <v>2075</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="14">
         <f>E7</f>
         <v>1675</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="20">
+      <c r="E19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0</v>
+      </c>
+      <c r="G19" s="14">
         <f>C7+G7+H7</f>
         <v>3830</v>
       </c>
-      <c r="G19" s="20">
-        <v>0</v>
-      </c>
-      <c r="H19" s="21">
+      <c r="H19" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0</v>
+      </c>
+      <c r="D20" s="16">
+        <f>E11</f>
+        <v>1070.8333333333301</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="14">
+        <v>0</v>
+      </c>
+      <c r="H20" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="20">
-        <v>0</v>
-      </c>
-      <c r="D20" s="20">
+      <c r="C21" s="14">
+        <v>0</v>
+      </c>
+      <c r="D21" s="14">
         <f>E9+E4+E8</f>
         <v>1500</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E21" s="14">
         <f>F4+F8+F9</f>
         <v>3380</v>
       </c>
-      <c r="F20" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="20">
-        <v>0</v>
-      </c>
-      <c r="H20" s="21">
+      <c r="F21" s="14">
+        <v>0</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="15">
         <f>K9</f>
         <v>1016</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="20">
-        <v>0</v>
-      </c>
-      <c r="D21" s="22">
-        <f>E11</f>
-        <v>1070.8333333333301</v>
-      </c>
-      <c r="E21" s="20">
-        <v>0</v>
-      </c>
-      <c r="F21" s="20">
-        <v>0</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="21">
-        <v>0</v>
-      </c>
-    </row>
     <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="23">
-        <v>0</v>
-      </c>
-      <c r="D22" s="23">
+      <c r="C22" s="17">
+        <v>0</v>
+      </c>
+      <c r="D22" s="17">
         <f>E12</f>
         <v>2000</v>
       </c>
-      <c r="E22" s="23">
-        <v>0</v>
-      </c>
-      <c r="F22" s="23">
+      <c r="E22" s="17">
+        <v>0</v>
+      </c>
+      <c r="F22" s="17">
         <f>H12</f>
         <v>1016</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="17">
         <f>H12</f>
         <v>1016</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="18" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP: add moving average for time series
</commit_message>
<xml_diff>
--- a/SeminarPaper/Model/input_data/ntc.xlsx
+++ b/SeminarPaper/Model/input_data/ntc.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86987AD-EB41-44D8-9A14-D327F6C0EA06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593D7068-8F29-4795-BAFA-EBADECFB303B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -537,13 +537,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
         <v>9</v>
       </c>
@@ -557,7 +557,7 @@
       <c r="J1" s="20"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -569,7 +569,7 @@
       <c r="J2" s="23"/>
       <c r="K2" s="24"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -619,7 +619,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -637,7 +637,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -661,7 +661,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -685,7 +685,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -703,7 +703,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
@@ -725,7 +725,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -743,7 +743,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -763,7 +763,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
@@ -783,8 +783,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
         <v>10</v>
       </c>
@@ -798,7 +798,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
@@ -810,7 +810,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
         <v>1</v>
@@ -831,7 +831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>1</v>
       </c>
@@ -855,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>2</v>
       </c>
@@ -882,7 +882,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>3</v>
       </c>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
@@ -932,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>4</v>
       </c>
@@ -958,7 +958,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
@@ -973,8 +973,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="17">
-        <f>H12</f>
-        <v>1016</v>
+        <v>0</v>
       </c>
       <c r="G22" s="17">
         <f>H12</f>
@@ -984,7 +983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:K2"/>

</xml_diff>